<commit_message>
Pushing changes from today
</commit_message>
<xml_diff>
--- a/pandas_column_formats.xlsx
+++ b/pandas_column_formats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Last Name, First Name</t>
   </si>
@@ -37,20 +37,19 @@
     <t>Number of Passengers you can take</t>
   </si>
   <si>
-    <t>Ireland, Ashley</t>
-  </si>
-  <si>
-    <t>McClung, Sheldon</t>
+    <t>Links, Kevin</t>
   </si>
   <si>
     <t>Nosar, Bryan</t>
   </si>
   <si>
-    <t>EDCI 502
-EDCI 509</t>
-  </si>
-  <si>
-    <t>EDCI 509</t>
+    <t>Scott, Spencer</t>
+  </si>
+  <si>
+    <t>EDCI 507</t>
+  </si>
+  <si>
+    <t>EDCI 501</t>
   </si>
   <si>
     <t>EDCI 501
@@ -58,18 +57,20 @@
 EDCI 507</t>
   </si>
   <si>
-    <t>T/TH 7:30:56 AM - 12:30:56 PM</t>
-  </si>
-  <si>
-    <t>T/TH 7:30:23 AM - 12:30:23 PM</t>
-  </si>
-  <si>
-    <t>M 7:30:21 AM - 3:30:21 PM
-T 7:30:21 AM - 3:30:21 PM
-W 7:30:21 AM - 3:30:21 PM</t>
-  </si>
-  <si>
-    <t>Elementary Education pK-6</t>
+    <t>M 7:30:02 AM - 3:30:02 PM</t>
+  </si>
+  <si>
+    <t>M 7:30:51 AM - 3:30:51 PM
+T 7:30:51 AM - 3:30:51 PM
+W 7:30:51 AM - 3:30:51 PM</t>
+  </si>
+  <si>
+    <t>M 7:30:27 AM - 3:30:27 PM
+T 7:30:27 AM - 3:30:27 PM
+W/TH/F 7:30:27 AM - 3:30:27 PM</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
   <si>
     <t>Elementary Education pK-6
@@ -77,15 +78,16 @@
 Foreign Language- French</t>
   </si>
   <si>
-    <t>Hugh Mercer Elementary School: 12</t>
-  </si>
-  <si>
-    <t>James Monroe High School: AP/DE/IB Biology
-Hugh Mercer Elementary School: Special Education: Adapted
-Livingston Elementary School: 4</t>
+    <t>Mountain View High School: AP/DE/IB Art</t>
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes and others</t>
   </si>
 </sst>
 </file>
@@ -503,11 +505,8 @@
       <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -523,6 +522,9 @@
       <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
@@ -540,11 +542,11 @@
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating reports is complete
</commit_message>
<xml_diff>
--- a/pandas_column_formats.xlsx
+++ b/pandas_column_formats.xlsx
@@ -14,80 +14,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
-  <si>
-    <t>Last Name, First Name</t>
-  </si>
-  <si>
-    <t>Courses</t>
-  </si>
-  <si>
-    <t>Days/Times</t>
-  </si>
-  <si>
-    <t>Endorsements</t>
-  </si>
-  <si>
-    <t>Previous Practica</t>
-  </si>
-  <si>
-    <t>Do you have a car?</t>
-  </si>
-  <si>
-    <t>Number of Passengers you can take</t>
-  </si>
-  <si>
-    <t>Links, Kevin</t>
-  </si>
-  <si>
-    <t>Nosar, Bryan</t>
-  </si>
-  <si>
-    <t>Scott, Spencer</t>
-  </si>
-  <si>
-    <t>EDCI 507</t>
-  </si>
-  <si>
-    <t>EDCI 501</t>
-  </si>
-  <si>
-    <t>EDCI 501
-EDCI 502
-EDCI 507</t>
-  </si>
-  <si>
-    <t>M 7:30:02 AM - 3:30:02 PM</t>
-  </si>
-  <si>
-    <t>M 7:30:51 AM - 3:30:51 PM
-T 7:30:51 AM - 3:30:51 PM
-W 7:30:51 AM - 3:30:51 PM</t>
-  </si>
-  <si>
-    <t>M 7:30:27 AM - 3:30:27 PM
-T 7:30:27 AM - 3:30:27 PM
-W/TH/F 7:30:27 AM - 3:30:27 PM</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Elementary Education pK-6
-English
-Foreign Language- French</t>
-  </si>
-  <si>
-    <t>Mountain View High School: AP/DE/IB Art</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes and others</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Assigned School</t>
+  </si>
+  <si>
+    <t>Host Teacher</t>
+  </si>
+  <si>
+    <t>Practicum Course</t>
+  </si>
+  <si>
+    <t>Practicum Day/Time</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Nosar</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Bryan</t>
+  </si>
+  <si>
+    <t>Spencer</t>
+  </si>
+  <si>
+    <t>Hugh Mercer Elementary School</t>
+  </si>
+  <si>
+    <t>A. G. Wright Middle School</t>
+  </si>
+  <si>
+    <t>Nosar, Cathy</t>
+  </si>
+  <si>
+    <t>Coleman, Henry</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Band III</t>
+  </si>
+  <si>
+    <t>M/T: 7:30:52 AM - 3:30:52 AM</t>
+  </si>
+  <si>
+    <t>M/T/W/Th/F: 7:30:03 AM - 3:30:03 AM</t>
+  </si>
+  <si>
+    <t>M/T: 7:30:06 AM - 3:30:06 AM</t>
   </si>
 </sst>
 </file>
@@ -104,6 +96,7 @@
     </font>
     <font>
       <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,18 +104,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -157,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -454,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -466,10 +453,9 @@
     <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="50.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
+    <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -488,65 +474,65 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G4" s="1">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>